<commit_message>
Update Foras Promineo CLR FM2 BOM.xlsx
</commit_message>
<xml_diff>
--- a/Foras-Promineo-CLR-FM2-Assembly-Files/Foras Promineo CLR FM2 BOM.xlsx
+++ b/Foras-Promineo-CLR-FM2-Assembly-Files/Foras Promineo CLR FM2 BOM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckkornowski\Documents\GitHub\Foras-Promineo-Camera-LED-Board\Foras-Promineo-CLR-FM2-Assembly-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4232D9CC-CB41-490B-821F-53BD04C23B47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61DD5E0-7313-4270-9A1B-95045ECB9AF7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26640" windowHeight="7980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26640" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foras Promineo CLR PCB" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>Source:</t>
   </si>
@@ -164,12 +164,24 @@
   </si>
   <si>
     <t xml:space="preserve">D1, D2, D3, D4, D5, D6, </t>
+  </si>
+  <si>
+    <t>Manufacturer 2</t>
+  </si>
+  <si>
+    <t>Manufacturer Part Number 2</t>
+  </si>
+  <si>
+    <t>Murata Electronics</t>
+  </si>
+  <si>
+    <t>GRM188C81C106MA73J</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1004,11 +1016,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,9 +1032,11 @@
     <col min="7" max="7" width="36.42578125" customWidth="1"/>
     <col min="10" max="10" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1030,7 +1044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -1038,7 +1052,7 @@
         <v>45177.567210648151</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -1046,7 +1060,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -1054,7 +1068,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -1062,7 +1076,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -1096,8 +1110,14 @@
       <c r="K6" t="s">
         <v>17</v>
       </c>
+      <c r="L6" t="s">
+        <v>48</v>
+      </c>
+      <c r="M6" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1126,7 +1146,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1154,8 +1174,14 @@
       <c r="K8" t="s">
         <v>28</v>
       </c>
+      <c r="L8" t="s">
+        <v>50</v>
+      </c>
+      <c r="M8" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1184,7 +1210,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1213,7 +1239,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>

</xml_diff>